<commit_message>
Updated codes in Financial page. added new test cases
</commit_message>
<xml_diff>
--- a/3PI/Testdata/Testdata.xlsx
+++ b/3PI/Testdata/Testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satheeshnair\PycharmProjects\3PI\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB792F9-20E9-4BA1-A3EC-2E506048F3B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCF2EC0-28E3-4485-9081-5B19C8E8681C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3630" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="admin" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Username</t>
   </si>
@@ -51,13 +51,58 @@
     <t>Value</t>
   </si>
   <si>
-    <t>test_1</t>
+    <t>test_selectOrderType</t>
+  </si>
+  <si>
+    <t>projectid</t>
+  </si>
+  <si>
+    <t>test_projectinfo</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>US - 2020</t>
+  </si>
+  <si>
+    <t>Capital Amount</t>
+  </si>
+  <si>
+    <t>Expense Amount</t>
+  </si>
+  <si>
+    <t>Quote Number</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>3D NETWORKS</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>test_order</t>
   </si>
   <si>
     <t>order</t>
   </si>
   <si>
-    <t>order value</t>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>upload</t>
+  </si>
+  <si>
+    <t>Dummyfor3PI</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>C:\Users\satheeshnair\Desktop\word\Dummyfor3PI.txt</t>
   </si>
 </sst>
 </file>
@@ -114,11 +159,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,17 +447,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="56.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -448,15 +496,113 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="4">
+        <v>98313</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Updated codes in Financial page. added new test cases Cleaned up code
</commit_message>
<xml_diff>
--- a/3PI/Testdata/Testdata.xlsx
+++ b/3PI/Testdata/Testdata.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satheeshnair\PycharmProjects\3PI\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCF2EC0-28E3-4485-9081-5B19C8E8681C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062327B0-A689-47E6-941E-6CF32A974AE0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="admin" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>Username</t>
   </si>
@@ -103,16 +109,66 @@
   </si>
   <si>
     <t>C:\Users\satheeshnair\Desktop\word\Dummyfor3PI.txt</t>
+  </si>
+  <si>
+    <t>test_shipto</t>
+  </si>
+  <si>
+    <t>satheeshnair</t>
+  </si>
+  <si>
+    <t>Recipient</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Office_phone</t>
+  </si>
+  <si>
+    <t>Expected_date</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Country_Ship</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Site_location</t>
+  </si>
+  <si>
+    <t>ADDISON</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>16175 ADDISON RD.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,10 +212,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -167,8 +224,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +542,7 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="1"/>
@@ -595,20 +658,101 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
+      <c r="A13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
+      <c r="A14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1231231231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="7">
+        <f ca="1">TODAY()</f>
+        <v>43984</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{ED23623B-8074-42DC-A052-4D77990F3EC4}"/>
+    <hyperlink ref="C13" r:id="rId2" display="satheeshnair@kpmg.com" xr:uid="{DD6E6E3D-56A7-4BCF-8ADD-EFD7DB67AA86}"/>
+    <hyperlink ref="C14" r:id="rId3" xr:uid="{3155A985-E3E5-438F-8531-8BE2AF8C368C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new test case Added new code to existing project
</commit_message>
<xml_diff>
--- a/3PI/Testdata/Testdata.xlsx
+++ b/3PI/Testdata/Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\satheeshnair\PycharmProjects\3PI\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062327B0-A689-47E6-941E-6CF32A974AE0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380DF97D-FCEE-438F-A858-C0306600E5FF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,112 +45,112 @@
     <t>test_login</t>
   </si>
   <si>
+    <t>TestCaseName</t>
+  </si>
+  <si>
+    <t>MethodName</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>test_selectOrderType</t>
+  </si>
+  <si>
+    <t>projectid</t>
+  </si>
+  <si>
+    <t>test_projectinfo</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>US - 2020</t>
+  </si>
+  <si>
+    <t>Capital Amount</t>
+  </si>
+  <si>
+    <t>Expense Amount</t>
+  </si>
+  <si>
+    <t>Quote Number</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>3D NETWORKS</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>test_order</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>upload</t>
+  </si>
+  <si>
+    <t>Dummyfor3PI</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>C:\Users\satheeshnair\Desktop\word\Dummyfor3PI.txt</t>
+  </si>
+  <si>
+    <t>test_shipto</t>
+  </si>
+  <si>
+    <t>Recipient</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Office_phone</t>
+  </si>
+  <si>
+    <t>Expected_date</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>Country_Ship</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Site_location</t>
+  </si>
+  <si>
+    <t>ADDISON</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>16175 ADDISON RD.</t>
+  </si>
+  <si>
     <t>Welcome26</t>
   </si>
   <si>
-    <t>TestCaseName</t>
-  </si>
-  <si>
-    <t>MethodName</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>test_selectOrderType</t>
-  </si>
-  <si>
-    <t>projectid</t>
-  </si>
-  <si>
-    <t>test_projectinfo</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>US - 2020</t>
-  </si>
-  <si>
-    <t>Capital Amount</t>
-  </si>
-  <si>
-    <t>Expense Amount</t>
-  </si>
-  <si>
-    <t>Quote Number</t>
-  </si>
-  <si>
-    <t>test123</t>
-  </si>
-  <si>
-    <t>3D NETWORKS</t>
-  </si>
-  <si>
-    <t>Supplier</t>
-  </si>
-  <si>
-    <t>test_order</t>
-  </si>
-  <si>
-    <t>order</t>
-  </si>
-  <si>
-    <t>Server</t>
-  </si>
-  <si>
-    <t>upload</t>
-  </si>
-  <si>
-    <t>Dummyfor3PI</t>
-  </si>
-  <si>
-    <t>path</t>
-  </si>
-  <si>
-    <t>C:\Users\satheeshnair\Desktop\word\Dummyfor3PI.txt</t>
-  </si>
-  <si>
-    <t>test_shipto</t>
-  </si>
-  <si>
-    <t>satheeshnair</t>
-  </si>
-  <si>
-    <t>Recipient</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Office_phone</t>
-  </si>
-  <si>
-    <t>Expected_date</t>
-  </si>
-  <si>
-    <t>Region</t>
+    <t>Satheesh Nair</t>
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>Country_Ship</t>
-  </si>
-  <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>Site_location</t>
-  </si>
-  <si>
-    <t>ADDISON</t>
-  </si>
-  <si>
-    <t>Street</t>
-  </si>
-  <si>
-    <t>16175 ADDISON RD.</t>
   </si>
 </sst>
 </file>
@@ -226,7 +226,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -513,7 +513,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,13 +526,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -555,26 +555,26 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="C5" s="4">
         <v>98313</v>
@@ -582,21 +582,21 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="4">
         <v>123</v>
@@ -604,10 +604,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
@@ -615,65 +615,65 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="C13" s="4" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>2</v>
@@ -681,10 +681,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" s="4">
         <v>1231231231</v>
@@ -692,58 +692,57 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="7">
-        <f ca="1">TODAY()</f>
-        <v>43984</v>
+        <v>12312020</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -753,6 +752,6 @@
     <hyperlink ref="C14" r:id="rId3" xr:uid="{3155A985-E3E5-438F-8531-8BE2AF8C368C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>